<commit_message>
Readme y Dashboard terminados, Proyecto finalizado
</commit_message>
<xml_diff>
--- a/data/homicidios_clean.xlsx
+++ b/data/homicidios_clean.xlsx
@@ -629,7 +629,7 @@
       </c>
       <c r="T2" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U2" t="inlineStr">
@@ -721,7 +721,7 @@
       </c>
       <c r="T3" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U3" t="inlineStr">
@@ -813,7 +813,7 @@
       </c>
       <c r="T4" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U4" t="inlineStr">
@@ -905,7 +905,7 @@
       </c>
       <c r="T5" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U5" t="inlineStr">
@@ -997,7 +997,7 @@
       </c>
       <c r="T6" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U6" t="inlineStr">
@@ -1089,7 +1089,7 @@
       </c>
       <c r="T7" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U7" t="inlineStr">
@@ -1181,7 +1181,7 @@
       </c>
       <c r="T8" t="inlineStr">
         <is>
-          <t>PASAJERO_ACOMPAÑANTE</t>
+          <t>Pasajero Acompañante</t>
         </is>
       </c>
       <c r="U8" t="inlineStr">
@@ -1273,7 +1273,7 @@
       </c>
       <c r="T9" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U9" t="inlineStr">
@@ -1365,7 +1365,7 @@
       </c>
       <c r="T10" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U10" t="inlineStr">
@@ -1641,7 +1641,7 @@
       </c>
       <c r="T13" t="inlineStr">
         <is>
-          <t>PASAJERO_ACOMPAÑANTE</t>
+          <t>Pasajero Acompañante</t>
         </is>
       </c>
       <c r="U13" t="inlineStr">
@@ -2009,7 +2009,7 @@
       </c>
       <c r="T17" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U17" t="inlineStr">
@@ -2101,7 +2101,7 @@
       </c>
       <c r="T18" t="inlineStr">
         <is>
-          <t>PASAJERO_ACOMPAÑANTE</t>
+          <t>Pasajero Acompañante</t>
         </is>
       </c>
       <c r="U18" t="inlineStr">
@@ -2193,7 +2193,7 @@
       </c>
       <c r="T19" t="inlineStr">
         <is>
-          <t>PASAJERO_ACOMPAÑANTE</t>
+          <t>Pasajero Acompañante</t>
         </is>
       </c>
       <c r="U19" t="inlineStr">
@@ -2285,7 +2285,7 @@
       </c>
       <c r="T20" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U20" t="inlineStr">
@@ -2377,7 +2377,7 @@
       </c>
       <c r="T21" t="inlineStr">
         <is>
-          <t>PASAJERO_ACOMPAÑANTE</t>
+          <t>Pasajero Acompañante</t>
         </is>
       </c>
       <c r="U21" t="inlineStr">
@@ -2653,7 +2653,7 @@
       </c>
       <c r="T24" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U24" t="inlineStr">
@@ -2837,7 +2837,7 @@
       </c>
       <c r="T26" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U26" t="inlineStr">
@@ -2929,7 +2929,7 @@
       </c>
       <c r="T27" t="inlineStr">
         <is>
-          <t>PASAJERO_ACOMPAÑANTE</t>
+          <t>Pasajero Acompañante</t>
         </is>
       </c>
       <c r="U27" t="inlineStr">
@@ -3021,7 +3021,7 @@
       </c>
       <c r="T28" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U28" t="inlineStr">
@@ -3205,7 +3205,7 @@
       </c>
       <c r="T30" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U30" t="inlineStr">
@@ -3297,7 +3297,7 @@
       </c>
       <c r="T31" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U31" t="inlineStr">
@@ -3389,7 +3389,7 @@
       </c>
       <c r="T32" t="inlineStr">
         <is>
-          <t>PASAJERO_ACOMPAÑANTE</t>
+          <t>Pasajero Acompañante</t>
         </is>
       </c>
       <c r="U32" t="inlineStr">
@@ -3398,7 +3398,7 @@
         </is>
       </c>
       <c r="V32" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="33">
@@ -3573,7 +3573,7 @@
       </c>
       <c r="T34" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U34" t="inlineStr">
@@ -3665,7 +3665,7 @@
       </c>
       <c r="T35" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U35" t="inlineStr">
@@ -3674,7 +3674,7 @@
         </is>
       </c>
       <c r="V35" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="36">
@@ -3858,7 +3858,7 @@
         </is>
       </c>
       <c r="V37" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="38">
@@ -4033,7 +4033,7 @@
       </c>
       <c r="T39" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U39" t="inlineStr">
@@ -4217,7 +4217,7 @@
       </c>
       <c r="T41" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U41" t="inlineStr">
@@ -4401,7 +4401,7 @@
       </c>
       <c r="T43" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U43" t="inlineStr">
@@ -4861,7 +4861,7 @@
       </c>
       <c r="T48" t="inlineStr">
         <is>
-          <t>PASAJERO_ACOMPAÑANTE</t>
+          <t>Pasajero Acompañante</t>
         </is>
       </c>
       <c r="U48" t="inlineStr">
@@ -4953,7 +4953,7 @@
       </c>
       <c r="T49" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U49" t="inlineStr">
@@ -5045,7 +5045,7 @@
       </c>
       <c r="T50" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U50" t="inlineStr">
@@ -5137,7 +5137,7 @@
       </c>
       <c r="T51" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U51" t="inlineStr">
@@ -5229,7 +5229,7 @@
       </c>
       <c r="T52" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U52" t="inlineStr">
@@ -5514,7 +5514,7 @@
         </is>
       </c>
       <c r="V55" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="56">
@@ -5597,7 +5597,7 @@
       </c>
       <c r="T56" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U56" t="inlineStr">
@@ -5689,7 +5689,7 @@
       </c>
       <c r="T57" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U57" t="inlineStr">
@@ -5781,7 +5781,7 @@
       </c>
       <c r="T58" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U58" t="inlineStr">
@@ -5873,7 +5873,7 @@
       </c>
       <c r="T59" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U59" t="inlineStr">
@@ -6333,7 +6333,7 @@
       </c>
       <c r="T64" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U64" t="inlineStr">
@@ -6701,7 +6701,7 @@
       </c>
       <c r="T68" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U68" t="inlineStr">
@@ -6793,7 +6793,7 @@
       </c>
       <c r="T69" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U69" t="inlineStr">
@@ -6885,7 +6885,7 @@
       </c>
       <c r="T70" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U70" t="inlineStr">
@@ -6977,7 +6977,7 @@
       </c>
       <c r="T71" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U71" t="inlineStr">
@@ -6986,7 +6986,7 @@
         </is>
       </c>
       <c r="V71" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="72">
@@ -7161,7 +7161,7 @@
       </c>
       <c r="T73" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U73" t="inlineStr">
@@ -7253,7 +7253,7 @@
       </c>
       <c r="T74" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U74" t="inlineStr">
@@ -7345,7 +7345,7 @@
       </c>
       <c r="T75" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U75" t="inlineStr">
@@ -7437,7 +7437,7 @@
       </c>
       <c r="T76" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U76" t="inlineStr">
@@ -7529,7 +7529,7 @@
       </c>
       <c r="T77" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U77" t="inlineStr">
@@ -7805,7 +7805,7 @@
       </c>
       <c r="T80" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U80" t="inlineStr">
@@ -7897,7 +7897,7 @@
       </c>
       <c r="T81" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U81" t="inlineStr">
@@ -8081,7 +8081,7 @@
       </c>
       <c r="T83" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U83" t="inlineStr">
@@ -8173,7 +8173,7 @@
       </c>
       <c r="T84" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U84" t="inlineStr">
@@ -8357,7 +8357,7 @@
       </c>
       <c r="T86" t="inlineStr">
         <is>
-          <t>CICLISTA</t>
+          <t>Ciclista</t>
         </is>
       </c>
       <c r="U86" t="inlineStr">
@@ -8449,7 +8449,7 @@
       </c>
       <c r="T87" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U87" t="inlineStr">
@@ -8541,7 +8541,7 @@
       </c>
       <c r="T88" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U88" t="inlineStr">
@@ -8633,7 +8633,7 @@
       </c>
       <c r="T89" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U89" t="inlineStr">
@@ -8725,7 +8725,7 @@
       </c>
       <c r="T90" t="inlineStr">
         <is>
-          <t>CICLISTA</t>
+          <t>Ciclista</t>
         </is>
       </c>
       <c r="U90" t="inlineStr">
@@ -8817,7 +8817,7 @@
       </c>
       <c r="T91" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U91" t="inlineStr">
@@ -9001,7 +9001,7 @@
       </c>
       <c r="T93" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U93" t="inlineStr">
@@ -9093,7 +9093,7 @@
       </c>
       <c r="T94" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U94" t="inlineStr">
@@ -9185,7 +9185,7 @@
       </c>
       <c r="T95" t="inlineStr">
         <is>
-          <t>PASAJERO_ACOMPAÑANTE</t>
+          <t>Pasajero Acompañante</t>
         </is>
       </c>
       <c r="U95" t="inlineStr">
@@ -9461,7 +9461,7 @@
       </c>
       <c r="T98" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U98" t="inlineStr">
@@ -9645,7 +9645,7 @@
       </c>
       <c r="T100" t="inlineStr">
         <is>
-          <t>PASAJERO_ACOMPAÑANTE</t>
+          <t>Pasajero Acompañante</t>
         </is>
       </c>
       <c r="U100" t="inlineStr">
@@ -9737,7 +9737,7 @@
       </c>
       <c r="T101" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U101" t="inlineStr">
@@ -9829,7 +9829,7 @@
       </c>
       <c r="T102" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U102" t="inlineStr">
@@ -10013,7 +10013,7 @@
       </c>
       <c r="T104" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U104" t="inlineStr">
@@ -10105,7 +10105,7 @@
       </c>
       <c r="T105" t="inlineStr">
         <is>
-          <t>CICLISTA</t>
+          <t>Ciclista</t>
         </is>
       </c>
       <c r="U105" t="inlineStr">
@@ -10197,7 +10197,7 @@
       </c>
       <c r="T106" t="inlineStr">
         <is>
-          <t>PASAJERO_ACOMPAÑANTE</t>
+          <t>Pasajero Acompañante</t>
         </is>
       </c>
       <c r="U106" t="inlineStr">
@@ -10289,7 +10289,7 @@
       </c>
       <c r="T107" t="inlineStr">
         <is>
-          <t>PASAJERO_ACOMPAÑANTE</t>
+          <t>Pasajero Acompañante</t>
         </is>
       </c>
       <c r="U107" t="inlineStr">
@@ -10381,7 +10381,7 @@
       </c>
       <c r="T108" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U108" t="inlineStr">
@@ -10473,7 +10473,7 @@
       </c>
       <c r="T109" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U109" t="inlineStr">
@@ -10657,7 +10657,7 @@
       </c>
       <c r="T111" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U111" t="inlineStr">
@@ -10841,7 +10841,7 @@
       </c>
       <c r="T113" t="inlineStr">
         <is>
-          <t>PASAJERO_ACOMPAÑANTE</t>
+          <t>Pasajero Acompañante</t>
         </is>
       </c>
       <c r="U113" t="inlineStr">
@@ -10933,7 +10933,7 @@
       </c>
       <c r="T114" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U114" t="inlineStr">
@@ -10942,7 +10942,7 @@
         </is>
       </c>
       <c r="V114" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="115">
@@ -11025,7 +11025,7 @@
       </c>
       <c r="T115" t="inlineStr">
         <is>
-          <t>PASAJERO_ACOMPAÑANTE</t>
+          <t>Pasajero Acompañante</t>
         </is>
       </c>
       <c r="U115" t="inlineStr">
@@ -11117,7 +11117,7 @@
       </c>
       <c r="T116" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U116" t="inlineStr">
@@ -11301,7 +11301,7 @@
       </c>
       <c r="T118" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U118" t="inlineStr">
@@ -11485,7 +11485,7 @@
       </c>
       <c r="T120" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U120" t="inlineStr">
@@ -11577,7 +11577,7 @@
       </c>
       <c r="T121" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U121" t="inlineStr">
@@ -11669,7 +11669,7 @@
       </c>
       <c r="T122" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U122" t="inlineStr">
@@ -11761,7 +11761,7 @@
       </c>
       <c r="T123" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U123" t="inlineStr">
@@ -12037,7 +12037,7 @@
       </c>
       <c r="T126" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U126" t="inlineStr">
@@ -12129,7 +12129,7 @@
       </c>
       <c r="T127" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U127" t="inlineStr">
@@ -12221,7 +12221,7 @@
       </c>
       <c r="T128" t="inlineStr">
         <is>
-          <t>CICLISTA</t>
+          <t>Ciclista</t>
         </is>
       </c>
       <c r="U128" t="inlineStr">
@@ -12313,7 +12313,7 @@
       </c>
       <c r="T129" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U129" t="inlineStr">
@@ -12405,7 +12405,7 @@
       </c>
       <c r="T130" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U130" t="inlineStr">
@@ -12497,7 +12497,7 @@
       </c>
       <c r="T131" t="inlineStr">
         <is>
-          <t>PASAJERO_ACOMPAÑANTE</t>
+          <t>Pasajero Acompañante</t>
         </is>
       </c>
       <c r="U131" t="inlineStr">
@@ -12589,7 +12589,7 @@
       </c>
       <c r="T132" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U132" t="inlineStr">
@@ -12681,7 +12681,7 @@
       </c>
       <c r="T133" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U133" t="inlineStr">
@@ -12782,7 +12782,7 @@
         </is>
       </c>
       <c r="V134" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="135">
@@ -12865,7 +12865,7 @@
       </c>
       <c r="T135" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U135" t="inlineStr">
@@ -13141,7 +13141,7 @@
       </c>
       <c r="T138" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U138" t="inlineStr">
@@ -13233,7 +13233,7 @@
       </c>
       <c r="T139" t="inlineStr">
         <is>
-          <t>PASAJERO_ACOMPAÑANTE</t>
+          <t>Pasajero Acompañante</t>
         </is>
       </c>
       <c r="U139" t="inlineStr">
@@ -13417,7 +13417,7 @@
       </c>
       <c r="T141" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U141" t="inlineStr">
@@ -13509,7 +13509,7 @@
       </c>
       <c r="T142" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U142" t="inlineStr">
@@ -13601,7 +13601,7 @@
       </c>
       <c r="T143" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U143" t="inlineStr">
@@ -13693,7 +13693,7 @@
       </c>
       <c r="T144" t="inlineStr">
         <is>
-          <t>PASAJERO_ACOMPAÑANTE</t>
+          <t>Pasajero Acompañante</t>
         </is>
       </c>
       <c r="U144" t="inlineStr">
@@ -13785,7 +13785,7 @@
       </c>
       <c r="T145" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U145" t="inlineStr">
@@ -13969,7 +13969,7 @@
       </c>
       <c r="T147" t="inlineStr">
         <is>
-          <t>PASAJERO_ACOMPAÑANTE</t>
+          <t>Pasajero Acompañante</t>
         </is>
       </c>
       <c r="U147" t="inlineStr">
@@ -14153,7 +14153,7 @@
       </c>
       <c r="T149" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U149" t="inlineStr">
@@ -14245,7 +14245,7 @@
       </c>
       <c r="T150" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U150" t="inlineStr">
@@ -14337,7 +14337,7 @@
       </c>
       <c r="T151" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U151" t="inlineStr">
@@ -14429,7 +14429,7 @@
       </c>
       <c r="T152" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U152" t="inlineStr">
@@ -14613,7 +14613,7 @@
       </c>
       <c r="T154" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U154" t="inlineStr">
@@ -14705,7 +14705,7 @@
       </c>
       <c r="T155" t="inlineStr">
         <is>
-          <t>PASAJERO_ACOMPAÑANTE</t>
+          <t>Pasajero Acompañante</t>
         </is>
       </c>
       <c r="U155" t="inlineStr">
@@ -14797,7 +14797,7 @@
       </c>
       <c r="T156" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U156" t="inlineStr">
@@ -14898,7 +14898,7 @@
         </is>
       </c>
       <c r="V157" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="158">
@@ -15073,7 +15073,7 @@
       </c>
       <c r="T159" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U159" t="inlineStr">
@@ -15165,7 +15165,7 @@
       </c>
       <c r="T160" t="inlineStr">
         <is>
-          <t>PASAJERO_ACOMPAÑANTE</t>
+          <t>Pasajero Acompañante</t>
         </is>
       </c>
       <c r="U160" t="inlineStr">
@@ -15257,7 +15257,7 @@
       </c>
       <c r="T161" t="inlineStr">
         <is>
-          <t>PASAJERO_ACOMPAÑANTE</t>
+          <t>Pasajero Acompañante</t>
         </is>
       </c>
       <c r="U161" t="inlineStr">
@@ -15349,7 +15349,7 @@
       </c>
       <c r="T162" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U162" t="inlineStr">
@@ -15533,7 +15533,7 @@
       </c>
       <c r="T164" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U164" t="inlineStr">
@@ -15625,7 +15625,7 @@
       </c>
       <c r="T165" t="inlineStr">
         <is>
-          <t>PASAJERO_ACOMPAÑANTE</t>
+          <t>Pasajero Acompañante</t>
         </is>
       </c>
       <c r="U165" t="inlineStr">
@@ -15717,7 +15717,7 @@
       </c>
       <c r="T166" t="inlineStr">
         <is>
-          <t>PASAJERO_ACOMPAÑANTE</t>
+          <t>Pasajero Acompañante</t>
         </is>
       </c>
       <c r="U166" t="inlineStr">
@@ -15809,7 +15809,7 @@
       </c>
       <c r="T167" t="inlineStr">
         <is>
-          <t>PASAJERO_ACOMPAÑANTE</t>
+          <t>Pasajero Acompañante</t>
         </is>
       </c>
       <c r="U167" t="inlineStr">
@@ -15818,7 +15818,7 @@
         </is>
       </c>
       <c r="V167" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="168">
@@ -15901,7 +15901,7 @@
       </c>
       <c r="T168" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U168" t="inlineStr">
@@ -15993,7 +15993,7 @@
       </c>
       <c r="T169" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U169" t="inlineStr">
@@ -16085,7 +16085,7 @@
       </c>
       <c r="T170" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U170" t="inlineStr">
@@ -16177,7 +16177,7 @@
       </c>
       <c r="T171" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U171" t="inlineStr">
@@ -16269,7 +16269,7 @@
       </c>
       <c r="T172" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U172" t="inlineStr">
@@ -16361,7 +16361,7 @@
       </c>
       <c r="T173" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U173" t="inlineStr">
@@ -16453,7 +16453,7 @@
       </c>
       <c r="T174" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U174" t="inlineStr">
@@ -16729,7 +16729,7 @@
       </c>
       <c r="T177" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U177" t="inlineStr">
@@ -16821,7 +16821,7 @@
       </c>
       <c r="T178" t="inlineStr">
         <is>
-          <t>PASAJERO_ACOMPAÑANTE</t>
+          <t>Pasajero Acompañante</t>
         </is>
       </c>
       <c r="U178" t="inlineStr">
@@ -16913,7 +16913,7 @@
       </c>
       <c r="T179" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U179" t="inlineStr">
@@ -17189,7 +17189,7 @@
       </c>
       <c r="T182" t="inlineStr">
         <is>
-          <t>PASAJERO_ACOMPAÑANTE</t>
+          <t>Pasajero Acompañante</t>
         </is>
       </c>
       <c r="U182" t="inlineStr">
@@ -17373,7 +17373,7 @@
       </c>
       <c r="T184" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U184" t="inlineStr">
@@ -17557,7 +17557,7 @@
       </c>
       <c r="T186" t="inlineStr">
         <is>
-          <t>PASAJERO_ACOMPAÑANTE</t>
+          <t>Pasajero Acompañante</t>
         </is>
       </c>
       <c r="U186" t="inlineStr">
@@ -17649,7 +17649,7 @@
       </c>
       <c r="T187" t="inlineStr">
         <is>
-          <t>CICLISTA</t>
+          <t>Ciclista</t>
         </is>
       </c>
       <c r="U187" t="inlineStr">
@@ -17833,7 +17833,7 @@
       </c>
       <c r="T189" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U189" t="inlineStr">
@@ -17925,7 +17925,7 @@
       </c>
       <c r="T190" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U190" t="inlineStr">
@@ -18017,7 +18017,7 @@
       </c>
       <c r="T191" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U191" t="inlineStr">
@@ -18201,7 +18201,7 @@
       </c>
       <c r="T193" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U193" t="inlineStr">
@@ -18293,7 +18293,7 @@
       </c>
       <c r="T194" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U194" t="inlineStr">
@@ -18569,7 +18569,7 @@
       </c>
       <c r="T197" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U197" t="inlineStr">
@@ -18661,7 +18661,7 @@
       </c>
       <c r="T198" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U198" t="inlineStr">
@@ -18937,7 +18937,7 @@
       </c>
       <c r="T201" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U201" t="inlineStr">
@@ -19581,7 +19581,7 @@
       </c>
       <c r="T208" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U208" t="inlineStr">
@@ -19774,7 +19774,7 @@
         </is>
       </c>
       <c r="V210" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="211">
@@ -19857,7 +19857,7 @@
       </c>
       <c r="T211" t="inlineStr">
         <is>
-          <t>CICLISTA</t>
+          <t>Ciclista</t>
         </is>
       </c>
       <c r="U211" t="inlineStr">
@@ -19949,7 +19949,7 @@
       </c>
       <c r="T212" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U212" t="inlineStr">
@@ -20225,7 +20225,7 @@
       </c>
       <c r="T215" t="inlineStr">
         <is>
-          <t>CICLISTA</t>
+          <t>Ciclista</t>
         </is>
       </c>
       <c r="U215" t="inlineStr">
@@ -20317,7 +20317,7 @@
       </c>
       <c r="T216" t="inlineStr">
         <is>
-          <t>PASAJERO_ACOMPAÑANTE</t>
+          <t>Pasajero Acompañante</t>
         </is>
       </c>
       <c r="U216" t="inlineStr">
@@ -20777,7 +20777,7 @@
       </c>
       <c r="T221" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U221" t="inlineStr">
@@ -20869,7 +20869,7 @@
       </c>
       <c r="T222" t="inlineStr">
         <is>
-          <t>PASAJERO_ACOMPAÑANTE</t>
+          <t>Pasajero Acompañante</t>
         </is>
       </c>
       <c r="U222" t="inlineStr">
@@ -20961,7 +20961,7 @@
       </c>
       <c r="T223" t="inlineStr">
         <is>
-          <t>PASAJERO_ACOMPAÑANTE</t>
+          <t>Pasajero Acompañante</t>
         </is>
       </c>
       <c r="U223" t="inlineStr">
@@ -21053,7 +21053,7 @@
       </c>
       <c r="T224" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U224" t="inlineStr">
@@ -21329,7 +21329,7 @@
       </c>
       <c r="T227" t="inlineStr">
         <is>
-          <t>PASAJERO_ACOMPAÑANTE</t>
+          <t>Pasajero Acompañante</t>
         </is>
       </c>
       <c r="U227" t="inlineStr">
@@ -21421,7 +21421,7 @@
       </c>
       <c r="T228" t="inlineStr">
         <is>
-          <t>PASAJERO_ACOMPAÑANTE</t>
+          <t>Pasajero Acompañante</t>
         </is>
       </c>
       <c r="U228" t="inlineStr">
@@ -21430,7 +21430,7 @@
         </is>
       </c>
       <c r="V228" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="229">
@@ -21605,7 +21605,7 @@
       </c>
       <c r="T230" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U230" t="inlineStr">
@@ -21697,7 +21697,7 @@
       </c>
       <c r="T231" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U231" t="inlineStr">
@@ -21789,7 +21789,7 @@
       </c>
       <c r="T232" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U232" t="inlineStr">
@@ -21881,7 +21881,7 @@
       </c>
       <c r="T233" t="inlineStr">
         <is>
-          <t>PASAJERO_ACOMPAÑANTE</t>
+          <t>Pasajero Acompañante</t>
         </is>
       </c>
       <c r="U233" t="inlineStr">
@@ -21973,7 +21973,7 @@
       </c>
       <c r="T234" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U234" t="inlineStr">
@@ -22157,7 +22157,7 @@
       </c>
       <c r="T236" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U236" t="inlineStr">
@@ -22249,7 +22249,7 @@
       </c>
       <c r="T237" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U237" t="inlineStr">
@@ -22341,7 +22341,7 @@
       </c>
       <c r="T238" t="inlineStr">
         <is>
-          <t>PASAJERO_ACOMPAÑANTE</t>
+          <t>Pasajero Acompañante</t>
         </is>
       </c>
       <c r="U238" t="inlineStr">
@@ -22433,7 +22433,7 @@
       </c>
       <c r="T239" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U239" t="inlineStr">
@@ -22525,7 +22525,7 @@
       </c>
       <c r="T240" t="inlineStr">
         <is>
-          <t>PASAJERO_ACOMPAÑANTE</t>
+          <t>Pasajero Acompañante</t>
         </is>
       </c>
       <c r="U240" t="inlineStr">
@@ -22709,7 +22709,7 @@
       </c>
       <c r="T242" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U242" t="inlineStr">
@@ -22801,7 +22801,7 @@
       </c>
       <c r="T243" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U243" t="inlineStr">
@@ -22893,7 +22893,7 @@
       </c>
       <c r="T244" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U244" t="inlineStr">
@@ -23077,7 +23077,7 @@
       </c>
       <c r="T246" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U246" t="inlineStr">
@@ -23353,7 +23353,7 @@
       </c>
       <c r="T249" t="inlineStr">
         <is>
-          <t>PASAJERO_ACOMPAÑANTE</t>
+          <t>Pasajero Acompañante</t>
         </is>
       </c>
       <c r="U249" t="inlineStr">
@@ -23445,7 +23445,7 @@
       </c>
       <c r="T250" t="inlineStr">
         <is>
-          <t>PASAJERO_ACOMPAÑANTE</t>
+          <t>Pasajero Acompañante</t>
         </is>
       </c>
       <c r="U250" t="inlineStr">
@@ -23629,7 +23629,7 @@
       </c>
       <c r="T252" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U252" t="inlineStr">
@@ -23721,7 +23721,7 @@
       </c>
       <c r="T253" t="inlineStr">
         <is>
-          <t>PASAJERO_ACOMPAÑANTE</t>
+          <t>Pasajero Acompañante</t>
         </is>
       </c>
       <c r="U253" t="inlineStr">
@@ -23813,7 +23813,7 @@
       </c>
       <c r="T254" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U254" t="inlineStr">
@@ -23905,7 +23905,7 @@
       </c>
       <c r="T255" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U255" t="inlineStr">
@@ -24282,7 +24282,7 @@
         </is>
       </c>
       <c r="V259" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="260">
@@ -24365,7 +24365,7 @@
       </c>
       <c r="T260" t="inlineStr">
         <is>
-          <t>CICLISTA</t>
+          <t>Ciclista</t>
         </is>
       </c>
       <c r="U260" t="inlineStr">
@@ -24457,7 +24457,7 @@
       </c>
       <c r="T261" t="inlineStr">
         <is>
-          <t>PASAJERO_ACOMPAÑANTE</t>
+          <t>Pasajero Acompañante</t>
         </is>
       </c>
       <c r="U261" t="inlineStr">
@@ -24466,7 +24466,7 @@
         </is>
       </c>
       <c r="V261" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="262">
@@ -24549,7 +24549,7 @@
       </c>
       <c r="T262" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U262" t="inlineStr">
@@ -24733,7 +24733,7 @@
       </c>
       <c r="T264" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U264" t="inlineStr">
@@ -24825,7 +24825,7 @@
       </c>
       <c r="T265" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U265" t="inlineStr">
@@ -24917,7 +24917,7 @@
       </c>
       <c r="T266" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U266" t="inlineStr">
@@ -25285,7 +25285,7 @@
       </c>
       <c r="T270" t="inlineStr">
         <is>
-          <t>CICLISTA</t>
+          <t>Ciclista</t>
         </is>
       </c>
       <c r="U270" t="inlineStr">
@@ -25469,7 +25469,7 @@
       </c>
       <c r="T272" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U272" t="inlineStr">
@@ -25653,7 +25653,7 @@
       </c>
       <c r="T274" t="inlineStr">
         <is>
-          <t>CICLISTA</t>
+          <t>Ciclista</t>
         </is>
       </c>
       <c r="U274" t="inlineStr">
@@ -25745,7 +25745,7 @@
       </c>
       <c r="T275" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U275" t="inlineStr">
@@ -25837,7 +25837,7 @@
       </c>
       <c r="T276" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U276" t="inlineStr">
@@ -25929,7 +25929,7 @@
       </c>
       <c r="T277" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U277" t="inlineStr">
@@ -26021,7 +26021,7 @@
       </c>
       <c r="T278" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U278" t="inlineStr">
@@ -26205,7 +26205,7 @@
       </c>
       <c r="T280" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U280" t="inlineStr">
@@ -26297,7 +26297,7 @@
       </c>
       <c r="T281" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U281" t="inlineStr">
@@ -26398,7 +26398,7 @@
         </is>
       </c>
       <c r="V282" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="283">
@@ -26481,7 +26481,7 @@
       </c>
       <c r="T283" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U283" t="inlineStr">
@@ -26573,7 +26573,7 @@
       </c>
       <c r="T284" t="inlineStr">
         <is>
-          <t>PASAJERO_ACOMPAÑANTE</t>
+          <t>Pasajero Acompañante</t>
         </is>
       </c>
       <c r="U284" t="inlineStr">
@@ -26665,7 +26665,7 @@
       </c>
       <c r="T285" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U285" t="inlineStr">
@@ -26849,7 +26849,7 @@
       </c>
       <c r="T287" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U287" t="inlineStr">
@@ -27033,7 +27033,7 @@
       </c>
       <c r="T289" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U289" t="inlineStr">
@@ -27217,7 +27217,7 @@
       </c>
       <c r="T291" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U291" t="inlineStr">
@@ -27309,7 +27309,7 @@
       </c>
       <c r="T292" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U292" t="inlineStr">
@@ -27585,7 +27585,7 @@
       </c>
       <c r="T295" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U295" t="inlineStr">
@@ -27677,7 +27677,7 @@
       </c>
       <c r="T296" t="inlineStr">
         <is>
-          <t>PASAJERO_ACOMPAÑANTE</t>
+          <t>Pasajero Acompañante</t>
         </is>
       </c>
       <c r="U296" t="inlineStr">
@@ -27953,7 +27953,7 @@
       </c>
       <c r="T299" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U299" t="inlineStr">
@@ -28045,7 +28045,7 @@
       </c>
       <c r="T300" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U300" t="inlineStr">
@@ -28137,7 +28137,7 @@
       </c>
       <c r="T301" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U301" t="inlineStr">
@@ -28321,7 +28321,7 @@
       </c>
       <c r="T303" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U303" t="inlineStr">
@@ -28597,7 +28597,7 @@
       </c>
       <c r="T306" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U306" t="inlineStr">
@@ -28974,7 +28974,7 @@
         </is>
       </c>
       <c r="V310" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="311">
@@ -29149,7 +29149,7 @@
       </c>
       <c r="T312" t="inlineStr">
         <is>
-          <t>PASAJERO_ACOMPAÑANTE</t>
+          <t>Pasajero Acompañante</t>
         </is>
       </c>
       <c r="U312" t="inlineStr">
@@ -29241,7 +29241,7 @@
       </c>
       <c r="T313" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U313" t="inlineStr">
@@ -29425,7 +29425,7 @@
       </c>
       <c r="T315" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U315" t="inlineStr">
@@ -30161,7 +30161,7 @@
       </c>
       <c r="T323" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U323" t="inlineStr">
@@ -30345,7 +30345,7 @@
       </c>
       <c r="T325" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U325" t="inlineStr">
@@ -30529,7 +30529,7 @@
       </c>
       <c r="T327" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U327" t="inlineStr">
@@ -30621,7 +30621,7 @@
       </c>
       <c r="T328" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U328" t="inlineStr">
@@ -30713,7 +30713,7 @@
       </c>
       <c r="T329" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U329" t="inlineStr">
@@ -30897,7 +30897,7 @@
       </c>
       <c r="T331" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U331" t="inlineStr">
@@ -31173,7 +31173,7 @@
       </c>
       <c r="T334" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U334" t="inlineStr">
@@ -31265,7 +31265,7 @@
       </c>
       <c r="T335" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U335" t="inlineStr">
@@ -31449,7 +31449,7 @@
       </c>
       <c r="T337" t="inlineStr">
         <is>
-          <t>PASAJERO_ACOMPAÑANTE</t>
+          <t>Pasajero Acompañante</t>
         </is>
       </c>
       <c r="U337" t="inlineStr">
@@ -31541,7 +31541,7 @@
       </c>
       <c r="T338" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U338" t="inlineStr">
@@ -31634,7 +31634,7 @@
       </c>
       <c r="T339" t="inlineStr">
         <is>
-          <t>CICLISTA</t>
+          <t>Ciclista</t>
         </is>
       </c>
       <c r="U339" t="inlineStr">
@@ -31726,7 +31726,7 @@
       </c>
       <c r="T340" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U340" t="inlineStr">
@@ -31818,7 +31818,7 @@
       </c>
       <c r="T341" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U341" t="inlineStr">
@@ -31827,7 +31827,7 @@
         </is>
       </c>
       <c r="V341" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="342">
@@ -31910,7 +31910,7 @@
       </c>
       <c r="T342" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U342" t="inlineStr">
@@ -32094,7 +32094,7 @@
       </c>
       <c r="T344" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U344" t="inlineStr">
@@ -32278,7 +32278,7 @@
       </c>
       <c r="T346" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U346" t="inlineStr">
@@ -32370,7 +32370,7 @@
       </c>
       <c r="T347" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U347" t="inlineStr">
@@ -32563,7 +32563,7 @@
         </is>
       </c>
       <c r="V349" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="350">
@@ -32830,7 +32830,7 @@
       </c>
       <c r="T352" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U352" t="inlineStr">
@@ -32922,7 +32922,7 @@
       </c>
       <c r="T353" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U353" t="inlineStr">
@@ -32931,7 +32931,7 @@
         </is>
       </c>
       <c r="V353" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="354">
@@ -33106,7 +33106,7 @@
       </c>
       <c r="T355" t="inlineStr">
         <is>
-          <t>PASAJERO_ACOMPAÑANTE</t>
+          <t>Pasajero Acompañante</t>
         </is>
       </c>
       <c r="U355" t="inlineStr">
@@ -33198,7 +33198,7 @@
       </c>
       <c r="T356" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U356" t="inlineStr">
@@ -33474,7 +33474,7 @@
       </c>
       <c r="T359" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U359" t="inlineStr">
@@ -33483,7 +33483,7 @@
         </is>
       </c>
       <c r="V359" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="360">
@@ -33658,7 +33658,7 @@
       </c>
       <c r="T361" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U361" t="inlineStr">
@@ -33750,7 +33750,7 @@
       </c>
       <c r="T362" t="inlineStr">
         <is>
-          <t>PASAJERO_ACOMPAÑANTE</t>
+          <t>Pasajero Acompañante</t>
         </is>
       </c>
       <c r="U362" t="inlineStr">
@@ -33842,7 +33842,7 @@
       </c>
       <c r="T363" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U363" t="inlineStr">
@@ -34026,7 +34026,7 @@
       </c>
       <c r="T365" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U365" t="inlineStr">
@@ -34118,7 +34118,7 @@
       </c>
       <c r="T366" t="inlineStr">
         <is>
-          <t>PASAJERO_ACOMPAÑANTE</t>
+          <t>Pasajero Acompañante</t>
         </is>
       </c>
       <c r="U366" t="inlineStr">
@@ -34302,7 +34302,7 @@
       </c>
       <c r="T368" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U368" t="inlineStr">
@@ -34394,7 +34394,7 @@
       </c>
       <c r="T369" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U369" t="inlineStr">
@@ -34486,7 +34486,7 @@
       </c>
       <c r="T370" t="inlineStr">
         <is>
-          <t>PASAJERO_ACOMPAÑANTE</t>
+          <t>Pasajero Acompañante</t>
         </is>
       </c>
       <c r="U370" t="inlineStr">
@@ -34670,7 +34670,7 @@
       </c>
       <c r="T372" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U372" t="inlineStr">
@@ -34679,7 +34679,7 @@
         </is>
       </c>
       <c r="V372" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="373">
@@ -34762,7 +34762,7 @@
       </c>
       <c r="T373" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U373" t="inlineStr">
@@ -34946,7 +34946,7 @@
       </c>
       <c r="T375" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U375" t="inlineStr">
@@ -35130,7 +35130,7 @@
       </c>
       <c r="T377" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U377" t="inlineStr">
@@ -35314,7 +35314,7 @@
       </c>
       <c r="T379" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U379" t="inlineStr">
@@ -35590,7 +35590,7 @@
       </c>
       <c r="T382" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U382" t="inlineStr">
@@ -35682,7 +35682,7 @@
       </c>
       <c r="T383" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U383" t="inlineStr">
@@ -35774,7 +35774,7 @@
       </c>
       <c r="T384" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U384" t="inlineStr">
@@ -35866,7 +35866,7 @@
       </c>
       <c r="T385" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U385" t="inlineStr">
@@ -36142,7 +36142,7 @@
       </c>
       <c r="T388" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U388" t="inlineStr">
@@ -36602,7 +36602,7 @@
       </c>
       <c r="T393" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U393" t="inlineStr">
@@ -36694,7 +36694,7 @@
       </c>
       <c r="T394" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U394" t="inlineStr">
@@ -36786,7 +36786,7 @@
       </c>
       <c r="T395" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U395" t="inlineStr">
@@ -36970,7 +36970,7 @@
       </c>
       <c r="T397" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U397" t="inlineStr">
@@ -37062,7 +37062,7 @@
       </c>
       <c r="T398" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U398" t="inlineStr">
@@ -37154,7 +37154,7 @@
       </c>
       <c r="T399" t="inlineStr">
         <is>
-          <t>PASAJERO_ACOMPAÑANTE</t>
+          <t>Pasajero Acompañante</t>
         </is>
       </c>
       <c r="U399" t="inlineStr">
@@ -37246,7 +37246,7 @@
       </c>
       <c r="T400" t="inlineStr">
         <is>
-          <t>PASAJERO_ACOMPAÑANTE</t>
+          <t>Pasajero Acompañante</t>
         </is>
       </c>
       <c r="U400" t="inlineStr">
@@ -37338,7 +37338,7 @@
       </c>
       <c r="T401" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U401" t="inlineStr">
@@ -37430,7 +37430,7 @@
       </c>
       <c r="T402" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U402" t="inlineStr">
@@ -37439,7 +37439,7 @@
         </is>
       </c>
       <c r="V402" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="403">
@@ -37522,7 +37522,7 @@
       </c>
       <c r="T403" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U403" t="inlineStr">
@@ -38074,7 +38074,7 @@
       </c>
       <c r="T409" t="inlineStr">
         <is>
-          <t>PASAJERO_ACOMPAÑANTE</t>
+          <t>Pasajero Acompañante</t>
         </is>
       </c>
       <c r="U409" t="inlineStr">
@@ -38166,7 +38166,7 @@
       </c>
       <c r="T410" t="inlineStr">
         <is>
-          <t>PASAJERO_ACOMPAÑANTE</t>
+          <t>Pasajero Acompañante</t>
         </is>
       </c>
       <c r="U410" t="inlineStr">
@@ -38258,7 +38258,7 @@
       </c>
       <c r="T411" t="inlineStr">
         <is>
-          <t>PASAJERO_ACOMPAÑANTE</t>
+          <t>Pasajero Acompañante</t>
         </is>
       </c>
       <c r="U411" t="inlineStr">
@@ -38350,7 +38350,7 @@
       </c>
       <c r="T412" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U412" t="inlineStr">
@@ -38534,7 +38534,7 @@
       </c>
       <c r="T414" t="inlineStr">
         <is>
-          <t>PASAJERO_ACOMPAÑANTE</t>
+          <t>Pasajero Acompañante</t>
         </is>
       </c>
       <c r="U414" t="inlineStr">
@@ -38626,7 +38626,7 @@
       </c>
       <c r="T415" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U415" t="inlineStr">
@@ -38718,7 +38718,7 @@
       </c>
       <c r="T416" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U416" t="inlineStr">
@@ -38810,7 +38810,7 @@
       </c>
       <c r="T417" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U417" t="inlineStr">
@@ -38902,7 +38902,7 @@
       </c>
       <c r="T418" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U418" t="inlineStr">
@@ -38994,7 +38994,7 @@
       </c>
       <c r="T419" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U419" t="inlineStr">
@@ -39086,7 +39086,7 @@
       </c>
       <c r="T420" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U420" t="inlineStr">
@@ -39270,7 +39270,7 @@
       </c>
       <c r="T422" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U422" t="inlineStr">
@@ -39362,7 +39362,7 @@
       </c>
       <c r="T423" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U423" t="inlineStr">
@@ -39454,7 +39454,7 @@
       </c>
       <c r="T424" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U424" t="inlineStr">
@@ -39555,7 +39555,7 @@
         </is>
       </c>
       <c r="V425" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="426">
@@ -39739,7 +39739,7 @@
         </is>
       </c>
       <c r="V427" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="428">
@@ -39822,7 +39822,7 @@
       </c>
       <c r="T428" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U428" t="inlineStr">
@@ -40006,7 +40006,7 @@
       </c>
       <c r="T430" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U430" t="inlineStr">
@@ -40098,7 +40098,7 @@
       </c>
       <c r="T431" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U431" t="inlineStr">
@@ -40190,7 +40190,7 @@
       </c>
       <c r="T432" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U432" t="inlineStr">
@@ -40282,7 +40282,7 @@
       </c>
       <c r="T433" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U433" t="inlineStr">
@@ -40466,7 +40466,7 @@
       </c>
       <c r="T435" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U435" t="inlineStr">
@@ -40475,7 +40475,7 @@
         </is>
       </c>
       <c r="V435" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="436">
@@ -40558,7 +40558,7 @@
       </c>
       <c r="T436" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U436" t="inlineStr">
@@ -40650,7 +40650,7 @@
       </c>
       <c r="T437" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U437" t="inlineStr">
@@ -40742,7 +40742,7 @@
       </c>
       <c r="T438" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U438" t="inlineStr">
@@ -40935,7 +40935,7 @@
         </is>
       </c>
       <c r="V440" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="441">
@@ -41018,7 +41018,7 @@
       </c>
       <c r="T441" t="inlineStr">
         <is>
-          <t>CICLISTA</t>
+          <t>Ciclista</t>
         </is>
       </c>
       <c r="U441" t="inlineStr">
@@ -41119,7 +41119,7 @@
         </is>
       </c>
       <c r="V442" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="443">
@@ -41202,7 +41202,7 @@
       </c>
       <c r="T443" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U443" t="inlineStr">
@@ -41294,7 +41294,7 @@
       </c>
       <c r="T444" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U444" t="inlineStr">
@@ -41386,7 +41386,7 @@
       </c>
       <c r="T445" t="inlineStr">
         <is>
-          <t>CICLISTA</t>
+          <t>Ciclista</t>
         </is>
       </c>
       <c r="U445" t="inlineStr">
@@ -41570,7 +41570,7 @@
       </c>
       <c r="T447" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U447" t="inlineStr">
@@ -41662,7 +41662,7 @@
       </c>
       <c r="T448" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U448" t="inlineStr">
@@ -41671,7 +41671,7 @@
         </is>
       </c>
       <c r="V448" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="449">
@@ -41846,7 +41846,7 @@
       </c>
       <c r="T450" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U450" t="inlineStr">
@@ -41938,7 +41938,7 @@
       </c>
       <c r="T451" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U451" t="inlineStr">
@@ -42122,7 +42122,7 @@
       </c>
       <c r="T453" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U453" t="inlineStr">
@@ -42214,7 +42214,7 @@
       </c>
       <c r="T454" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U454" t="inlineStr">
@@ -42306,7 +42306,7 @@
       </c>
       <c r="T455" t="inlineStr">
         <is>
-          <t>PASAJERO_ACOMPAÑANTE</t>
+          <t>Pasajero Acompañante</t>
         </is>
       </c>
       <c r="U455" t="inlineStr">
@@ -42490,7 +42490,7 @@
       </c>
       <c r="T457" t="inlineStr">
         <is>
-          <t>CICLISTA</t>
+          <t>Ciclista</t>
         </is>
       </c>
       <c r="U457" t="inlineStr">
@@ -42499,7 +42499,7 @@
         </is>
       </c>
       <c r="V457" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="458">
@@ -42674,7 +42674,7 @@
       </c>
       <c r="T459" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U459" t="inlineStr">
@@ -42766,7 +42766,7 @@
       </c>
       <c r="T460" t="inlineStr">
         <is>
-          <t>PASAJERO_ACOMPAÑANTE</t>
+          <t>Pasajero Acompañante</t>
         </is>
       </c>
       <c r="U460" t="inlineStr">
@@ -42950,7 +42950,7 @@
       </c>
       <c r="T462" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U462" t="inlineStr">
@@ -43134,7 +43134,7 @@
       </c>
       <c r="T464" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U464" t="inlineStr">
@@ -43226,7 +43226,7 @@
       </c>
       <c r="T465" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U465" t="inlineStr">
@@ -43318,7 +43318,7 @@
       </c>
       <c r="T466" t="inlineStr">
         <is>
-          <t>PASAJERO_ACOMPAÑANTE</t>
+          <t>Pasajero Acompañante</t>
         </is>
       </c>
       <c r="U466" t="inlineStr">
@@ -43410,7 +43410,7 @@
       </c>
       <c r="T467" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U467" t="inlineStr">
@@ -43502,7 +43502,7 @@
       </c>
       <c r="T468" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U468" t="inlineStr">
@@ -43778,7 +43778,7 @@
       </c>
       <c r="T471" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U471" t="inlineStr">
@@ -43870,7 +43870,7 @@
       </c>
       <c r="T472" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U472" t="inlineStr">
@@ -44238,7 +44238,7 @@
       </c>
       <c r="T476" t="inlineStr">
         <is>
-          <t>PASAJERO_ACOMPAÑANTE</t>
+          <t>Pasajero Acompañante</t>
         </is>
       </c>
       <c r="U476" t="inlineStr">
@@ -44247,7 +44247,7 @@
         </is>
       </c>
       <c r="V476" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="477">
@@ -44330,7 +44330,7 @@
       </c>
       <c r="T477" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U477" t="inlineStr">
@@ -44606,7 +44606,7 @@
       </c>
       <c r="T480" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U480" t="inlineStr">
@@ -44698,7 +44698,7 @@
       </c>
       <c r="T481" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U481" t="inlineStr">
@@ -44790,7 +44790,7 @@
       </c>
       <c r="T482" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U482" t="inlineStr">
@@ -44882,7 +44882,7 @@
       </c>
       <c r="T483" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U483" t="inlineStr">
@@ -44983,7 +44983,7 @@
         </is>
       </c>
       <c r="V484" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="485">
@@ -45066,7 +45066,7 @@
       </c>
       <c r="T485" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U485" t="inlineStr">
@@ -45158,7 +45158,7 @@
       </c>
       <c r="T486" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U486" t="inlineStr">
@@ -45250,7 +45250,7 @@
       </c>
       <c r="T487" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U487" t="inlineStr">
@@ -45342,7 +45342,7 @@
       </c>
       <c r="T488" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U488" t="inlineStr">
@@ -45434,7 +45434,7 @@
       </c>
       <c r="T489" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U489" t="inlineStr">
@@ -45710,7 +45710,7 @@
       </c>
       <c r="T492" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U492" t="inlineStr">
@@ -45894,7 +45894,7 @@
       </c>
       <c r="T494" t="inlineStr">
         <is>
-          <t>CICLISTA</t>
+          <t>Ciclista</t>
         </is>
       </c>
       <c r="U494" t="inlineStr">
@@ -45986,7 +45986,7 @@
       </c>
       <c r="T495" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U495" t="inlineStr">
@@ -46078,7 +46078,7 @@
       </c>
       <c r="T496" t="inlineStr">
         <is>
-          <t>CICLISTA</t>
+          <t>Ciclista</t>
         </is>
       </c>
       <c r="U496" t="inlineStr">
@@ -46170,7 +46170,7 @@
       </c>
       <c r="T497" t="inlineStr">
         <is>
-          <t>CICLISTA</t>
+          <t>Ciclista</t>
         </is>
       </c>
       <c r="U497" t="inlineStr">
@@ -46262,7 +46262,7 @@
       </c>
       <c r="T498" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U498" t="inlineStr">
@@ -46354,7 +46354,7 @@
       </c>
       <c r="T499" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U499" t="inlineStr">
@@ -46906,7 +46906,7 @@
       </c>
       <c r="T505" t="inlineStr">
         <is>
-          <t>CICLISTA</t>
+          <t>Ciclista</t>
         </is>
       </c>
       <c r="U505" t="inlineStr">
@@ -46998,7 +46998,7 @@
       </c>
       <c r="T506" t="inlineStr">
         <is>
-          <t>PASAJERO_ACOMPAÑANTE</t>
+          <t>Pasajero Acompañante</t>
         </is>
       </c>
       <c r="U506" t="inlineStr">
@@ -47007,7 +47007,7 @@
         </is>
       </c>
       <c r="V506" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="507">
@@ -47090,7 +47090,7 @@
       </c>
       <c r="T507" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U507" t="inlineStr">
@@ -47099,7 +47099,7 @@
         </is>
       </c>
       <c r="V507" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="508">
@@ -47274,7 +47274,7 @@
       </c>
       <c r="T509" t="inlineStr">
         <is>
-          <t>PASAJERO_ACOMPAÑANTE</t>
+          <t>Pasajero Acompañante</t>
         </is>
       </c>
       <c r="U509" t="inlineStr">
@@ -47366,7 +47366,7 @@
       </c>
       <c r="T510" t="inlineStr">
         <is>
-          <t>PASAJERO_ACOMPAÑANTE</t>
+          <t>Pasajero Acompañante</t>
         </is>
       </c>
       <c r="U510" t="inlineStr">
@@ -47458,7 +47458,7 @@
       </c>
       <c r="T511" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U511" t="inlineStr">
@@ -47550,7 +47550,7 @@
       </c>
       <c r="T512" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U512" t="inlineStr">
@@ -47642,7 +47642,7 @@
       </c>
       <c r="T513" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U513" t="inlineStr">
@@ -47734,7 +47734,7 @@
       </c>
       <c r="T514" t="inlineStr">
         <is>
-          <t>PASAJERO_ACOMPAÑANTE</t>
+          <t>Pasajero Acompañante</t>
         </is>
       </c>
       <c r="U514" t="inlineStr">
@@ -48010,7 +48010,7 @@
       </c>
       <c r="T517" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U517" t="inlineStr">
@@ -48286,7 +48286,7 @@
       </c>
       <c r="T520" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U520" t="inlineStr">
@@ -48378,7 +48378,7 @@
       </c>
       <c r="T521" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U521" t="inlineStr">
@@ -48562,7 +48562,7 @@
       </c>
       <c r="T523" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U523" t="inlineStr">
@@ -48746,7 +48746,7 @@
       </c>
       <c r="T525" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U525" t="inlineStr">
@@ -48755,7 +48755,7 @@
         </is>
       </c>
       <c r="V525" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="526">
@@ -48838,7 +48838,7 @@
       </c>
       <c r="T526" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U526" t="inlineStr">
@@ -49114,7 +49114,7 @@
       </c>
       <c r="T529" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U529" t="inlineStr">
@@ -49123,7 +49123,7 @@
         </is>
       </c>
       <c r="V529" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="530">
@@ -49206,7 +49206,7 @@
       </c>
       <c r="T530" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U530" t="inlineStr">
@@ -49399,7 +49399,7 @@
         </is>
       </c>
       <c r="V532" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="533">
@@ -49482,7 +49482,7 @@
       </c>
       <c r="T533" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U533" t="inlineStr">
@@ -49850,7 +49850,7 @@
       </c>
       <c r="T537" t="inlineStr">
         <is>
-          <t>PASAJERO_ACOMPAÑANTE</t>
+          <t>Pasajero Acompañante</t>
         </is>
       </c>
       <c r="U537" t="inlineStr">
@@ -49942,7 +49942,7 @@
       </c>
       <c r="T538" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U538" t="inlineStr">
@@ -50034,7 +50034,7 @@
       </c>
       <c r="T539" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U539" t="inlineStr">
@@ -50135,7 +50135,7 @@
         </is>
       </c>
       <c r="V540" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="541">
@@ -50494,7 +50494,7 @@
       </c>
       <c r="T544" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U544" t="inlineStr">
@@ -50586,7 +50586,7 @@
       </c>
       <c r="T545" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U545" t="inlineStr">
@@ -50678,7 +50678,7 @@
       </c>
       <c r="T546" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U546" t="inlineStr">
@@ -50770,7 +50770,7 @@
       </c>
       <c r="T547" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U547" t="inlineStr">
@@ -50871,7 +50871,7 @@
         </is>
       </c>
       <c r="V548" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="549">
@@ -50954,7 +50954,7 @@
       </c>
       <c r="T549" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U549" t="inlineStr">
@@ -51230,7 +51230,7 @@
       </c>
       <c r="T552" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U552" t="inlineStr">
@@ -51322,7 +51322,7 @@
       </c>
       <c r="T553" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U553" t="inlineStr">
@@ -51414,7 +51414,7 @@
       </c>
       <c r="T554" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U554" t="inlineStr">
@@ -51423,7 +51423,7 @@
         </is>
       </c>
       <c r="V554" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="555">
@@ -51506,7 +51506,7 @@
       </c>
       <c r="T555" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U555" t="inlineStr">
@@ -51782,7 +51782,7 @@
       </c>
       <c r="T558" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U558" t="inlineStr">
@@ -51874,7 +51874,7 @@
       </c>
       <c r="T559" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U559" t="inlineStr">
@@ -51966,7 +51966,7 @@
       </c>
       <c r="T560" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U560" t="inlineStr">
@@ -52150,7 +52150,7 @@
       </c>
       <c r="T562" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U562" t="inlineStr">
@@ -52426,7 +52426,7 @@
       </c>
       <c r="T565" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U565" t="inlineStr">
@@ -52518,7 +52518,7 @@
       </c>
       <c r="T566" t="inlineStr">
         <is>
-          <t>CICLISTA</t>
+          <t>Ciclista</t>
         </is>
       </c>
       <c r="U566" t="inlineStr">
@@ -52610,7 +52610,7 @@
       </c>
       <c r="T567" t="inlineStr">
         <is>
-          <t>PASAJERO_ACOMPAÑANTE</t>
+          <t>Pasajero Acompañante</t>
         </is>
       </c>
       <c r="U567" t="inlineStr">
@@ -52702,7 +52702,7 @@
       </c>
       <c r="T568" t="inlineStr">
         <is>
-          <t>CICLISTA</t>
+          <t>Ciclista</t>
         </is>
       </c>
       <c r="U568" t="inlineStr">
@@ -52886,7 +52886,7 @@
       </c>
       <c r="T570" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U570" t="inlineStr">
@@ -53346,7 +53346,7 @@
       </c>
       <c r="T575" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U575" t="inlineStr">
@@ -53438,7 +53438,7 @@
       </c>
       <c r="T576" t="inlineStr">
         <is>
-          <t>CICLISTA</t>
+          <t>Ciclista</t>
         </is>
       </c>
       <c r="U576" t="inlineStr">
@@ -53530,7 +53530,7 @@
       </c>
       <c r="T577" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U577" t="inlineStr">
@@ -53622,7 +53622,7 @@
       </c>
       <c r="T578" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U578" t="inlineStr">
@@ -53806,7 +53806,7 @@
       </c>
       <c r="T580" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U580" t="inlineStr">
@@ -53898,7 +53898,7 @@
       </c>
       <c r="T581" t="inlineStr">
         <is>
-          <t>PASAJERO_ACOMPAÑANTE</t>
+          <t>Pasajero Acompañante</t>
         </is>
       </c>
       <c r="U581" t="inlineStr">
@@ -54174,7 +54174,7 @@
       </c>
       <c r="T584" t="inlineStr">
         <is>
-          <t>CICLISTA</t>
+          <t>Ciclista</t>
         </is>
       </c>
       <c r="U584" t="inlineStr">
@@ -54266,7 +54266,7 @@
       </c>
       <c r="T585" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U585" t="inlineStr">
@@ -54358,7 +54358,7 @@
       </c>
       <c r="T586" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U586" t="inlineStr">
@@ -54542,7 +54542,7 @@
       </c>
       <c r="T588" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U588" t="inlineStr">
@@ -54634,7 +54634,7 @@
       </c>
       <c r="T589" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U589" t="inlineStr">
@@ -54726,7 +54726,7 @@
       </c>
       <c r="T590" t="inlineStr">
         <is>
-          <t>PASAJERO_ACOMPAÑANTE</t>
+          <t>Pasajero Acompañante</t>
         </is>
       </c>
       <c r="U590" t="inlineStr">
@@ -54818,7 +54818,7 @@
       </c>
       <c r="T591" t="inlineStr">
         <is>
-          <t>CICLISTA</t>
+          <t>Ciclista</t>
         </is>
       </c>
       <c r="U591" t="inlineStr">
@@ -54910,7 +54910,7 @@
       </c>
       <c r="T592" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U592" t="inlineStr">
@@ -55002,7 +55002,7 @@
       </c>
       <c r="T593" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U593" t="inlineStr">
@@ -55094,7 +55094,7 @@
       </c>
       <c r="T594" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U594" t="inlineStr">
@@ -55186,7 +55186,7 @@
       </c>
       <c r="T595" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U595" t="inlineStr">
@@ -55462,7 +55462,7 @@
       </c>
       <c r="T598" t="inlineStr">
         <is>
-          <t>PASAJERO_ACOMPAÑANTE</t>
+          <t>Pasajero Acompañante</t>
         </is>
       </c>
       <c r="U598" t="inlineStr">
@@ -55554,7 +55554,7 @@
       </c>
       <c r="T599" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U599" t="inlineStr">
@@ -55738,7 +55738,7 @@
       </c>
       <c r="T601" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U601" t="inlineStr">
@@ -55830,7 +55830,7 @@
       </c>
       <c r="T602" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U602" t="inlineStr">
@@ -56023,7 +56023,7 @@
         </is>
       </c>
       <c r="V604" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="605">
@@ -56106,7 +56106,7 @@
       </c>
       <c r="T605" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U605" t="inlineStr">
@@ -56290,7 +56290,7 @@
       </c>
       <c r="T607" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U607" t="inlineStr">
@@ -56382,7 +56382,7 @@
       </c>
       <c r="T608" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U608" t="inlineStr">
@@ -56474,7 +56474,7 @@
       </c>
       <c r="T609" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U609" t="inlineStr">
@@ -56658,7 +56658,7 @@
       </c>
       <c r="T611" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U611" t="inlineStr">
@@ -56759,7 +56759,7 @@
         </is>
       </c>
       <c r="V612" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="613">
@@ -56842,7 +56842,7 @@
       </c>
       <c r="T613" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U613" t="inlineStr">
@@ -56934,7 +56934,7 @@
       </c>
       <c r="T614" t="inlineStr">
         <is>
-          <t>PASAJERO_ACOMPAÑANTE</t>
+          <t>Pasajero Acompañante</t>
         </is>
       </c>
       <c r="U614" t="inlineStr">
@@ -57026,7 +57026,7 @@
       </c>
       <c r="T615" t="inlineStr">
         <is>
-          <t>CICLISTA</t>
+          <t>Ciclista</t>
         </is>
       </c>
       <c r="U615" t="inlineStr">
@@ -57118,7 +57118,7 @@
       </c>
       <c r="T616" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U616" t="inlineStr">
@@ -57210,7 +57210,7 @@
       </c>
       <c r="T617" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U617" t="inlineStr">
@@ -57302,7 +57302,7 @@
       </c>
       <c r="T618" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U618" t="inlineStr">
@@ -57403,7 +57403,7 @@
         </is>
       </c>
       <c r="V619" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="620">
@@ -57486,7 +57486,7 @@
       </c>
       <c r="T620" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U620" t="inlineStr">
@@ -57854,7 +57854,7 @@
       </c>
       <c r="T624" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U624" t="inlineStr">
@@ -57946,7 +57946,7 @@
       </c>
       <c r="T625" t="inlineStr">
         <is>
-          <t>PASAJERO_ACOMPAÑANTE</t>
+          <t>Pasajero Acompañante</t>
         </is>
       </c>
       <c r="U625" t="inlineStr">
@@ -58038,7 +58038,7 @@
       </c>
       <c r="T626" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U626" t="inlineStr">
@@ -58130,7 +58130,7 @@
       </c>
       <c r="T627" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U627" t="inlineStr">
@@ -58314,7 +58314,7 @@
       </c>
       <c r="T629" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U629" t="inlineStr">
@@ -58406,7 +58406,7 @@
       </c>
       <c r="T630" t="inlineStr">
         <is>
-          <t>CICLISTA</t>
+          <t>Ciclista</t>
         </is>
       </c>
       <c r="U630" t="inlineStr">
@@ -58498,7 +58498,7 @@
       </c>
       <c r="T631" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U631" t="inlineStr">
@@ -58866,7 +58866,7 @@
       </c>
       <c r="T635" t="inlineStr">
         <is>
-          <t>PASAJERO_ACOMPAÑANTE</t>
+          <t>Pasajero Acompañante</t>
         </is>
       </c>
       <c r="U635" t="inlineStr">
@@ -58958,7 +58958,7 @@
       </c>
       <c r="T636" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U636" t="inlineStr">
@@ -59050,7 +59050,7 @@
       </c>
       <c r="T637" t="inlineStr">
         <is>
-          <t>PASAJERO_ACOMPAÑANTE</t>
+          <t>Pasajero Acompañante</t>
         </is>
       </c>
       <c r="U637" t="inlineStr">
@@ -59142,7 +59142,7 @@
       </c>
       <c r="T638" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U638" t="inlineStr">
@@ -59234,7 +59234,7 @@
       </c>
       <c r="T639" t="inlineStr">
         <is>
-          <t>CICLISTA</t>
+          <t>Ciclista</t>
         </is>
       </c>
       <c r="U639" t="inlineStr">
@@ -59326,7 +59326,7 @@
       </c>
       <c r="T640" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U640" t="inlineStr">
@@ -59418,7 +59418,7 @@
       </c>
       <c r="T641" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U641" t="inlineStr">
@@ -59602,7 +59602,7 @@
       </c>
       <c r="T643" t="inlineStr">
         <is>
-          <t>PASAJERO_ACOMPAÑANTE</t>
+          <t>Pasajero Acompañante</t>
         </is>
       </c>
       <c r="U643" t="inlineStr">
@@ -59786,7 +59786,7 @@
       </c>
       <c r="T645" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U645" t="inlineStr">
@@ -59878,7 +59878,7 @@
       </c>
       <c r="T646" t="inlineStr">
         <is>
-          <t>PASAJERO_ACOMPAÑANTE</t>
+          <t>Pasajero Acompañante</t>
         </is>
       </c>
       <c r="U646" t="inlineStr">
@@ -59970,7 +59970,7 @@
       </c>
       <c r="T647" t="inlineStr">
         <is>
-          <t>CICLISTA</t>
+          <t>Ciclista</t>
         </is>
       </c>
       <c r="U647" t="inlineStr">
@@ -60062,7 +60062,7 @@
       </c>
       <c r="T648" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U648" t="inlineStr">
@@ -60246,7 +60246,7 @@
       </c>
       <c r="T650" t="inlineStr">
         <is>
-          <t>PASAJERO_ACOMPAÑANTE</t>
+          <t>Pasajero Acompañante</t>
         </is>
       </c>
       <c r="U650" t="inlineStr">
@@ -60522,7 +60522,7 @@
       </c>
       <c r="T653" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U653" t="inlineStr">
@@ -60614,7 +60614,7 @@
       </c>
       <c r="T654" t="inlineStr">
         <is>
-          <t>PASAJERO_ACOMPAÑANTE</t>
+          <t>Pasajero Acompañante</t>
         </is>
       </c>
       <c r="U654" t="inlineStr">
@@ -60982,7 +60982,7 @@
       </c>
       <c r="T658" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U658" t="inlineStr">
@@ -61074,7 +61074,7 @@
       </c>
       <c r="T659" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U659" t="inlineStr">
@@ -61258,7 +61258,7 @@
       </c>
       <c r="T661" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U661" t="inlineStr">
@@ -61534,7 +61534,7 @@
       </c>
       <c r="T664" t="inlineStr">
         <is>
-          <t>CICLISTA</t>
+          <t>Ciclista</t>
         </is>
       </c>
       <c r="U664" t="inlineStr">
@@ -61626,7 +61626,7 @@
       </c>
       <c r="T665" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U665" t="inlineStr">
@@ -61810,7 +61810,7 @@
       </c>
       <c r="T667" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U667" t="inlineStr">
@@ -61902,7 +61902,7 @@
       </c>
       <c r="T668" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U668" t="inlineStr">
@@ -61994,7 +61994,7 @@
       </c>
       <c r="T669" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U669" t="inlineStr">
@@ -62095,7 +62095,7 @@
         </is>
       </c>
       <c r="V670" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="671">
@@ -62178,7 +62178,7 @@
       </c>
       <c r="T671" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U671" t="inlineStr">
@@ -62270,7 +62270,7 @@
       </c>
       <c r="T672" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U672" t="inlineStr">
@@ -62362,7 +62362,7 @@
       </c>
       <c r="T673" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U673" t="inlineStr">
@@ -62454,7 +62454,7 @@
       </c>
       <c r="T674" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U674" t="inlineStr">
@@ -62546,7 +62546,7 @@
       </c>
       <c r="T675" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U675" t="inlineStr">
@@ -62638,7 +62638,7 @@
       </c>
       <c r="T676" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U676" t="inlineStr">
@@ -62914,7 +62914,7 @@
       </c>
       <c r="T679" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U679" t="inlineStr">
@@ -63006,7 +63006,7 @@
       </c>
       <c r="T680" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U680" t="inlineStr">
@@ -63190,7 +63190,7 @@
       </c>
       <c r="T682" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U682" t="inlineStr">
@@ -63374,7 +63374,7 @@
       </c>
       <c r="T684" t="inlineStr">
         <is>
-          <t>PASAJERO_ACOMPAÑANTE</t>
+          <t>Pasajero Acompañante</t>
         </is>
       </c>
       <c r="U684" t="inlineStr">
@@ -63466,7 +63466,7 @@
       </c>
       <c r="T685" t="inlineStr">
         <is>
-          <t>PASAJERO_ACOMPAÑANTE</t>
+          <t>Pasajero Acompañante</t>
         </is>
       </c>
       <c r="U685" t="inlineStr">
@@ -63558,7 +63558,7 @@
       </c>
       <c r="T686" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U686" t="inlineStr">
@@ -63650,7 +63650,7 @@
       </c>
       <c r="T687" t="inlineStr">
         <is>
-          <t>CONDUCTOR</t>
+          <t>Conductor</t>
         </is>
       </c>
       <c r="U687" t="inlineStr">
@@ -63742,7 +63742,7 @@
       </c>
       <c r="T688" t="inlineStr">
         <is>
-          <t>CICLISTA</t>
+          <t>Ciclista</t>
         </is>
       </c>
       <c r="U688" t="inlineStr">

</xml_diff>